<commit_message>
feat(backend): ability to link overlapping referense which happens in composite keys (beta) and ability to indicate column positions
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/cohort_catalogue.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/cohort_catalogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/IdeaProjects/emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1416DA-5F66-084C-B9C4-08E591FAAB10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B338E53-DE82-D147-8806-305B3488B1BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
@@ -1518,7 +1518,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1580,6 +1580,21 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1664,7 +1679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1695,6 +1710,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2028,8 +2045,8 @@
   <dimension ref="A1:I74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H53" sqref="H53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5611,21 +5628,21 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E1" sqref="E1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.83203125" customWidth="1"/>
     <col min="9" max="9" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.6640625" customWidth="1"/>
+    <col min="10" max="10" width="29.6640625" style="27" customWidth="1"/>
     <col min="11" max="11" width="34.5" customWidth="1"/>
     <col min="12" max="12" width="56.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -5634,20 +5651,20 @@
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="26" t="s">
+        <v>449</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>447</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
@@ -5658,7 +5675,7 @@
       <c r="I1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="26" t="s">
         <v>451</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -5672,22 +5689,22 @@
       <c r="A2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2" s="27" t="str">
         <f>A2</f>
         <v>LifeCycle</v>
       </c>
       <c r="C2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="27" t="str">
+        <f t="shared" ref="E2:E13" si="0">A2</f>
+        <v>LifeCycle</v>
+      </c>
+      <c r="F2" t="s">
         <v>421</v>
-      </c>
-      <c r="D2" t="str">
-        <f>A2</f>
-        <v>LifeCycle</v>
-      </c>
-      <c r="E2" t="s">
-        <v>417</v>
-      </c>
-      <c r="F2" t="s">
-        <v>69</v>
       </c>
       <c r="G2" t="s">
         <v>71</v>
@@ -5698,7 +5715,7 @@
       <c r="I2" t="s">
         <v>84</v>
       </c>
-      <c r="J2" t="str">
+      <c r="J2" s="27" t="str">
         <f>A2</f>
         <v>LifeCycle</v>
       </c>
@@ -5710,22 +5727,22 @@
       <c r="A3" t="s">
         <v>68</v>
       </c>
-      <c r="B3" t="str">
-        <f t="shared" ref="B3:B13" si="0">A3</f>
-        <v>LifeCycle</v>
-      </c>
-      <c r="C3" t="s">
-        <v>421</v>
-      </c>
-      <c r="D3" t="str">
+      <c r="B3" s="27" t="str">
         <f>A3</f>
         <v>LifeCycle</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C3" t="s">
         <v>417</v>
       </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>LifeCycle</v>
+      </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>421</v>
       </c>
       <c r="G3" t="s">
         <v>71</v>
@@ -5736,7 +5753,7 @@
       <c r="I3" t="s">
         <v>188</v>
       </c>
-      <c r="J3" t="str">
+      <c r="J3" s="27" t="str">
         <f t="shared" ref="J3:J13" si="1">A3</f>
         <v>LifeCycle</v>
       </c>
@@ -5748,22 +5765,22 @@
       <c r="A4" t="s">
         <v>68</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B4" s="27" t="str">
+        <f t="shared" ref="B4:B10" si="2">A4</f>
+        <v>LifeCycle</v>
+      </c>
+      <c r="C4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LifeCycle</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>421</v>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" ref="D3:D13" si="2">A4</f>
-        <v>LifeCycle</v>
-      </c>
-      <c r="E4" t="s">
-        <v>417</v>
-      </c>
-      <c r="F4" t="s">
-        <v>74</v>
       </c>
       <c r="G4" t="s">
         <v>71</v>
@@ -5774,7 +5791,7 @@
       <c r="I4" t="s">
         <v>187</v>
       </c>
-      <c r="J4" t="str">
+      <c r="J4" s="27" t="str">
         <f t="shared" si="1"/>
         <v>LifeCycle</v>
       </c>
@@ -5786,22 +5803,22 @@
       <c r="A5" t="s">
         <v>347</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v>CHOP</v>
+      </c>
+      <c r="C5" t="s">
+        <v>417</v>
+      </c>
+      <c r="D5" t="s">
+        <v>377</v>
+      </c>
+      <c r="E5" s="27" t="str">
         <f t="shared" si="0"/>
         <v>CHOP</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>421</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="2"/>
-        <v>CHOP</v>
-      </c>
-      <c r="E5" t="s">
-        <v>417</v>
-      </c>
-      <c r="F5" t="s">
-        <v>377</v>
       </c>
       <c r="G5" t="s">
         <v>71</v>
@@ -5812,7 +5829,7 @@
       <c r="I5" t="s">
         <v>188</v>
       </c>
-      <c r="J5" t="str">
+      <c r="J5" s="27" t="str">
         <f t="shared" si="1"/>
         <v>CHOP</v>
       </c>
@@ -5821,22 +5838,22 @@
       <c r="A6" t="s">
         <v>347</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B6" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v>CHOP</v>
+      </c>
+      <c r="C6" t="s">
+        <v>417</v>
+      </c>
+      <c r="D6" t="s">
+        <v>378</v>
+      </c>
+      <c r="E6" s="27" t="str">
         <f t="shared" si="0"/>
         <v>CHOP</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
         <v>421</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="2"/>
-        <v>CHOP</v>
-      </c>
-      <c r="E6" t="s">
-        <v>417</v>
-      </c>
-      <c r="F6" t="s">
-        <v>378</v>
       </c>
       <c r="G6" t="s">
         <v>71</v>
@@ -5847,7 +5864,7 @@
       <c r="I6" t="s">
         <v>187</v>
       </c>
-      <c r="J6" t="str">
+      <c r="J6" s="27" t="str">
         <f t="shared" si="1"/>
         <v>CHOP</v>
       </c>
@@ -5856,22 +5873,22 @@
       <c r="A7" t="s">
         <v>356</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B7" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v>ELFE</v>
+      </c>
+      <c r="C7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D7" t="s">
+        <v>379</v>
+      </c>
+      <c r="E7" s="27" t="str">
         <f t="shared" si="0"/>
         <v>ELFE</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
         <v>421</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="2"/>
-        <v>ELFE</v>
-      </c>
-      <c r="E7" t="s">
-        <v>417</v>
-      </c>
-      <c r="F7" t="s">
-        <v>379</v>
       </c>
       <c r="G7" t="s">
         <v>71</v>
@@ -5882,7 +5899,7 @@
       <c r="I7" t="s">
         <v>187</v>
       </c>
-      <c r="J7" t="str">
+      <c r="J7" s="27" t="str">
         <f t="shared" si="1"/>
         <v>ELFE</v>
       </c>
@@ -5891,22 +5908,22 @@
       <c r="A8" t="s">
         <v>356</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B8" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v>ELFE</v>
+      </c>
+      <c r="C8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D8" t="s">
+        <v>380</v>
+      </c>
+      <c r="E8" s="27" t="str">
         <f t="shared" si="0"/>
         <v>ELFE</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" t="s">
         <v>421</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="2"/>
-        <v>ELFE</v>
-      </c>
-      <c r="E8" t="s">
-        <v>417</v>
-      </c>
-      <c r="F8" t="s">
-        <v>380</v>
       </c>
       <c r="G8" t="s">
         <v>71</v>
@@ -5917,7 +5934,7 @@
       <c r="I8" t="s">
         <v>187</v>
       </c>
-      <c r="J8" t="str">
+      <c r="J8" s="27" t="str">
         <f t="shared" si="1"/>
         <v>ELFE</v>
       </c>
@@ -5926,22 +5943,22 @@
       <c r="A9" t="s">
         <v>363</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B9" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v>GenR</v>
+      </c>
+      <c r="C9" t="s">
+        <v>417</v>
+      </c>
+      <c r="D9" t="s">
+        <v>381</v>
+      </c>
+      <c r="E9" s="27" t="str">
         <f t="shared" si="0"/>
         <v>GenR</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
         <v>421</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="2"/>
-        <v>GenR</v>
-      </c>
-      <c r="E9" t="s">
-        <v>417</v>
-      </c>
-      <c r="F9" t="s">
-        <v>381</v>
       </c>
       <c r="G9" t="s">
         <v>71</v>
@@ -5952,7 +5969,7 @@
       <c r="I9" t="s">
         <v>188</v>
       </c>
-      <c r="J9" t="str">
+      <c r="J9" s="27" t="str">
         <f t="shared" si="1"/>
         <v>GenR</v>
       </c>
@@ -5961,22 +5978,22 @@
       <c r="A10" t="s">
         <v>363</v>
       </c>
-      <c r="B10" t="str">
+      <c r="B10" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v>GenR</v>
+      </c>
+      <c r="C10" t="s">
+        <v>417</v>
+      </c>
+      <c r="D10" t="s">
+        <v>382</v>
+      </c>
+      <c r="E10" s="27" t="str">
         <f t="shared" si="0"/>
         <v>GenR</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" t="s">
         <v>421</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" si="2"/>
-        <v>GenR</v>
-      </c>
-      <c r="E10" t="s">
-        <v>417</v>
-      </c>
-      <c r="F10" t="s">
-        <v>382</v>
       </c>
       <c r="G10" t="s">
         <v>71</v>
@@ -5987,7 +6004,7 @@
       <c r="I10" t="s">
         <v>187</v>
       </c>
-      <c r="J10" t="str">
+      <c r="J10" s="27" t="str">
         <f t="shared" si="1"/>
         <v>GenR</v>
       </c>
@@ -5996,15 +6013,15 @@
       <c r="A11" t="s">
         <v>370</v>
       </c>
-      <c r="B11" t="str">
+      <c r="D11" t="s">
+        <v>383</v>
+      </c>
+      <c r="E11" s="27" t="str">
         <f t="shared" si="0"/>
         <v>NINFEA</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
         <v>421</v>
-      </c>
-      <c r="F11" t="s">
-        <v>383</v>
       </c>
       <c r="G11" t="s">
         <v>71</v>
@@ -6015,7 +6032,7 @@
       <c r="I11" t="s">
         <v>188</v>
       </c>
-      <c r="J11" t="str">
+      <c r="J11" s="27" t="str">
         <f t="shared" si="1"/>
         <v>NINFEA</v>
       </c>
@@ -6024,15 +6041,15 @@
       <c r="A12" t="s">
         <v>370</v>
       </c>
-      <c r="B12" t="str">
+      <c r="D12" t="s">
+        <v>384</v>
+      </c>
+      <c r="E12" s="27" t="str">
         <f t="shared" si="0"/>
         <v>NINFEA</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
         <v>421</v>
-      </c>
-      <c r="F12" t="s">
-        <v>384</v>
       </c>
       <c r="G12" t="s">
         <v>71</v>
@@ -6043,7 +6060,7 @@
       <c r="I12" t="s">
         <v>84</v>
       </c>
-      <c r="J12" t="str">
+      <c r="J12" s="27" t="str">
         <f t="shared" si="1"/>
         <v>NINFEA</v>
       </c>
@@ -6052,15 +6069,15 @@
       <c r="A13" t="s">
         <v>370</v>
       </c>
-      <c r="B13" t="str">
+      <c r="D13" t="s">
+        <v>385</v>
+      </c>
+      <c r="E13" s="27" t="str">
         <f t="shared" si="0"/>
         <v>NINFEA</v>
       </c>
-      <c r="C13" t="s">
+      <c r="F13" t="s">
         <v>421</v>
-      </c>
-      <c r="F13" t="s">
-        <v>385</v>
       </c>
       <c r="G13" t="s">
         <v>71</v>
@@ -6071,7 +6088,7 @@
       <c r="I13" t="s">
         <v>187</v>
       </c>
-      <c r="J13" t="str">
+      <c r="J13" s="27" t="str">
         <f t="shared" si="1"/>
         <v>NINFEA</v>
       </c>
@@ -6087,15 +6104,17 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" customWidth="1"/>
-    <col min="6" max="9" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" style="27" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
+    <col min="7" max="8" width="23.83203125" style="27" customWidth="1"/>
+    <col min="9" max="9" width="23.83203125" customWidth="1"/>
     <col min="10" max="10" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6103,7 +6122,7 @@
       <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="26" t="s">
         <v>449</v>
       </c>
       <c r="C1" s="7" t="s">
@@ -6112,16 +6131,16 @@
       <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="26" t="s">
         <v>447</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="26" t="s">
         <v>453</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="26" t="s">
         <v>454</v>
       </c>
       <c r="I1" s="7" t="s">
@@ -6135,7 +6154,7 @@
       <c r="A2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="6" t="str">
+      <c r="B2" s="27" t="str">
         <f>A2</f>
         <v>LifeCycle</v>
       </c>
@@ -6145,18 +6164,18 @@
       <c r="D2" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="E2" s="6" t="str">
+      <c r="E2" s="27" t="str">
         <f>A2</f>
         <v>LifeCycle</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="G2" s="6" t="str">
+      <c r="G2" s="27" t="str">
         <f>A2</f>
         <v>LifeCycle</v>
       </c>
-      <c r="H2" s="6" t="str">
+      <c r="H2" s="27" t="str">
         <f>A2</f>
         <v>LifeCycle</v>
       </c>
@@ -6171,7 +6190,7 @@
       <c r="A3" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="6" t="str">
+      <c r="B3" s="27" t="str">
         <f t="shared" ref="B3:B4" si="0">A3</f>
         <v>LifeCycle</v>
       </c>
@@ -6181,18 +6200,18 @@
       <c r="D3" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="E3" s="6" t="str">
+      <c r="E3" s="27" t="str">
         <f t="shared" ref="E3:E5" si="1">A3</f>
         <v>LifeCycle</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="G3" s="6" t="str">
+      <c r="G3" s="27" t="str">
         <f t="shared" ref="G3:G4" si="2">A3</f>
         <v>LifeCycle</v>
       </c>
-      <c r="H3" s="6" t="str">
+      <c r="H3" s="27" t="str">
         <f t="shared" ref="H3:H4" si="3">A3</f>
         <v>LifeCycle</v>
       </c>
@@ -6207,7 +6226,7 @@
       <c r="A4" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="6" t="str">
+      <c r="B4" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LifeCycle</v>
       </c>
@@ -6217,18 +6236,18 @@
       <c r="D4" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="E4" s="6" t="str">
+      <c r="E4" s="27" t="str">
         <f t="shared" si="1"/>
         <v>LifeCycle</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="G4" s="6" t="str">
+      <c r="G4" s="27" t="str">
         <f t="shared" si="2"/>
         <v>LifeCycle</v>
       </c>
-      <c r="H4" s="6" t="str">
+      <c r="H4" s="27" t="str">
         <f t="shared" si="3"/>
         <v>LifeCycle</v>
       </c>
@@ -6243,7 +6262,7 @@
       <c r="A5" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="6" t="str">
+      <c r="B5" s="27" t="str">
         <f t="shared" ref="B5" si="4">A5</f>
         <v>LifeCycle</v>
       </c>
@@ -6253,18 +6272,18 @@
       <c r="D5" t="s">
         <v>419</v>
       </c>
-      <c r="E5" s="6" t="str">
+      <c r="E5" s="27" t="str">
         <f t="shared" si="1"/>
         <v>LifeCycle</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="G5" s="6" t="str">
+      <c r="G5" s="27" t="str">
         <f t="shared" ref="G5" si="5">A5</f>
         <v>LifeCycle</v>
       </c>
-      <c r="H5" s="6" t="str">
+      <c r="H5" s="27" t="str">
         <f t="shared" ref="H5" si="6">A5</f>
         <v>LifeCycle</v>
       </c>
@@ -6344,17 +6363,18 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="22.83203125" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" style="27" customWidth="1"/>
     <col min="3" max="3" width="19.83203125" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.1640625" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="27" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" style="27" customWidth="1"/>
     <col min="8" max="8" width="24.5" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
     <col min="11" max="11" width="80.33203125" bestFit="1" customWidth="1"/>
@@ -6365,7 +6385,7 @@
       <c r="A1" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="26" t="s">
         <v>458</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -6377,10 +6397,10 @@
       <c r="E1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="26" t="s">
         <v>460</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="26" t="s">
         <v>461</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -6403,7 +6423,7 @@
       <c r="A2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2" s="27" t="str">
         <f>A2</f>
         <v>LifeCycle</v>
       </c>
@@ -6433,7 +6453,7 @@
       <c r="A3" t="s">
         <v>68</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3" s="27" t="str">
         <f t="shared" ref="B3:B15" si="0">A3</f>
         <v>LifeCycle</v>
       </c>
@@ -6446,11 +6466,11 @@
       <c r="E3" t="s">
         <v>347</v>
       </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F15" si="1">E3</f>
+      <c r="F3" s="27" t="str">
+        <f t="shared" ref="F3:F13" si="1">E3</f>
         <v>CHOP</v>
       </c>
-      <c r="G3" t="str">
+      <c r="G3" s="27" t="str">
         <f>E3</f>
         <v>CHOP</v>
       </c>
@@ -6474,7 +6494,7 @@
       <c r="A4" t="s">
         <v>68</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B4" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LifeCycle</v>
       </c>
@@ -6487,11 +6507,11 @@
       <c r="E4" t="s">
         <v>347</v>
       </c>
-      <c r="F4" t="str">
+      <c r="F4" s="27" t="str">
         <f t="shared" si="1"/>
         <v>CHOP</v>
       </c>
-      <c r="G4" t="str">
+      <c r="G4" s="27" t="str">
         <f>E4</f>
         <v>CHOP</v>
       </c>
@@ -6515,7 +6535,7 @@
       <c r="A5" t="s">
         <v>68</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LifeCycle</v>
       </c>
@@ -6542,7 +6562,7 @@
       <c r="A6" t="s">
         <v>68</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B6" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LifeCycle</v>
       </c>
@@ -6555,11 +6575,11 @@
       <c r="E6" t="s">
         <v>356</v>
       </c>
-      <c r="F6" t="str">
+      <c r="F6" s="27" t="str">
         <f t="shared" si="1"/>
         <v>ELFE</v>
       </c>
-      <c r="G6" t="str">
+      <c r="G6" s="27" t="str">
         <f>E6</f>
         <v>ELFE</v>
       </c>
@@ -6583,7 +6603,7 @@
       <c r="A7" t="s">
         <v>68</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B7" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LifeCycle</v>
       </c>
@@ -6596,11 +6616,11 @@
       <c r="E7" t="s">
         <v>356</v>
       </c>
-      <c r="F7" t="str">
+      <c r="F7" s="27" t="str">
         <f t="shared" si="1"/>
         <v>ELFE</v>
       </c>
-      <c r="G7" t="str">
+      <c r="G7" s="27" t="str">
         <f>E7</f>
         <v>ELFE</v>
       </c>
@@ -6624,7 +6644,7 @@
       <c r="A8" t="s">
         <v>68</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B8" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LifeCycle</v>
       </c>
@@ -6637,11 +6657,11 @@
       <c r="E8" t="s">
         <v>363</v>
       </c>
-      <c r="F8" t="str">
+      <c r="F8" s="27" t="str">
         <f t="shared" si="1"/>
         <v>GenR</v>
       </c>
-      <c r="G8" t="str">
+      <c r="G8" s="27" t="str">
         <f>E8</f>
         <v>GenR</v>
       </c>
@@ -6665,7 +6685,7 @@
       <c r="A9" t="s">
         <v>68</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B9" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LifeCycle</v>
       </c>
@@ -6678,11 +6698,11 @@
       <c r="E9" t="s">
         <v>363</v>
       </c>
-      <c r="F9" t="str">
+      <c r="F9" s="27" t="str">
         <f t="shared" si="1"/>
         <v>GenR</v>
       </c>
-      <c r="G9" t="str">
+      <c r="G9" s="27" t="str">
         <f>E9</f>
         <v>GenR</v>
       </c>
@@ -6706,7 +6726,7 @@
       <c r="A10" t="s">
         <v>68</v>
       </c>
-      <c r="B10" t="str">
+      <c r="B10" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LifeCycle</v>
       </c>
@@ -6736,7 +6756,7 @@
       <c r="A11" t="s">
         <v>68</v>
       </c>
-      <c r="B11" t="str">
+      <c r="B11" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LifeCycle</v>
       </c>
@@ -6749,7 +6769,7 @@
       <c r="E11" t="s">
         <v>370</v>
       </c>
-      <c r="F11" t="str">
+      <c r="F11" s="27" t="str">
         <f t="shared" si="1"/>
         <v>NINFEA</v>
       </c>
@@ -6770,7 +6790,7 @@
       <c r="A12" t="s">
         <v>68</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B12" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LifeCycle</v>
       </c>
@@ -6783,7 +6803,7 @@
       <c r="E12" t="s">
         <v>370</v>
       </c>
-      <c r="F12" t="str">
+      <c r="F12" s="27" t="str">
         <f t="shared" si="1"/>
         <v>NINFEA</v>
       </c>
@@ -6804,7 +6824,7 @@
       <c r="A13" t="s">
         <v>68</v>
       </c>
-      <c r="B13" t="str">
+      <c r="B13" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LifeCycle</v>
       </c>
@@ -6817,7 +6837,7 @@
       <c r="E13" t="s">
         <v>370</v>
       </c>
-      <c r="F13" t="str">
+      <c r="F13" s="27" t="str">
         <f t="shared" si="1"/>
         <v>NINFEA</v>
       </c>
@@ -6838,7 +6858,7 @@
       <c r="A14" t="s">
         <v>68</v>
       </c>
-      <c r="B14" t="str">
+      <c r="B14" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LifeCycle</v>
       </c>
@@ -6859,7 +6879,7 @@
       <c r="A15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B15" t="str">
+      <c r="B15" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LifeCycle</v>
       </c>
@@ -6872,8 +6892,8 @@
       <c r="E15" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="F15"/>
-      <c r="G15"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
       <c r="H15"/>
       <c r="J15" s="4" t="s">
         <v>395</v>

</xml_diff>

<commit_message>
feature: introduce file upload in graphql and UI forms
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/cohort_catalogue.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/cohort_catalogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/IdeaProjects/emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B338E53-DE82-D147-8806-305B3488B1BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C15A798-357B-5740-B429-7D909D7E6373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <sheet name="HarmonizationStatus" sheetId="7" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">molgenis!$A$1:$J$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">molgenis!$A$1:$J$58</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="468">
   <si>
     <t>name</t>
   </si>
@@ -1512,6 +1512,12 @@
   </si>
   <si>
     <t>ontologyTerm</t>
+  </si>
+  <si>
+    <t>CollectionDocuments</t>
+  </si>
+  <si>
+    <t>file</t>
   </si>
 </sst>
 </file>
@@ -2042,11 +2048,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E080B8D-E59C-EC4A-8043-87277F816BB8}">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2228,234 +2234,222 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="E11" s="12">
+        <v>1</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>467</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E14" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+    <row r="15" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E15" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
+    <row r="16" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D16" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+    <row r="17" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D17" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
+    <row r="18" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="12" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D18" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
+    <row r="19" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
         <v>414</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I19" s="17" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
+    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
         <v>414</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>443</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E20" s="11">
         <v>1</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>443</v>
-      </c>
-      <c r="E17" s="11">
-        <v>1</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="11">
-        <v>1</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>443</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>414</v>
-      </c>
-      <c r="I20" s="17" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>24</v>
+        <v>414</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>443</v>
       </c>
+      <c r="E21" s="11">
+        <v>1</v>
+      </c>
       <c r="F21" s="11" t="s">
-        <v>66</v>
+        <v>25</v>
+      </c>
+      <c r="H21" s="11" t="b">
+        <v>1</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>5</v>
+        <v>436</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>24</v>
+        <v>414</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="11" t="b">
+      <c r="E22" s="11">
         <v>1</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>24</v>
+        <v>414</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>443</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>409</v>
+        <v>22</v>
       </c>
       <c r="H23" s="11" t="b">
         <v>1</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>442</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>410</v>
-      </c>
-      <c r="H24" s="11" t="b">
-        <v>1</v>
+      <c r="B24" s="17" t="s">
+        <v>414</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2463,19 +2457,16 @@
         <v>24</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>443</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="11" t="b">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>435</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2483,7 +2474,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>7</v>
@@ -2497,16 +2488,19 @@
         <v>24</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>7</v>
+        <v>443</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>409</v>
       </c>
       <c r="H27" s="11" t="b">
         <v>1</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2514,19 +2508,16 @@
         <v>24</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>444</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>443</v>
+        <v>43</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>442</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>432</v>
+        <v>410</v>
       </c>
       <c r="H28" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2534,280 +2525,283 @@
         <v>24</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>445</v>
+        <v>9</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>443</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>432</v>
+        <v>8</v>
       </c>
       <c r="H29" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="I29" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="17" t="s">
-        <v>408</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>414</v>
-      </c>
-      <c r="I30" s="17" t="s">
-        <v>429</v>
+      <c r="I29" s="11" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="11" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>444</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="H32" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="H33" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="17" t="s">
         <v>408</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="B34" s="17" t="s">
+        <v>414</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>403</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D35" s="11" t="s">
         <v>443</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F35" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="23" t="s">
+    <row r="36" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C36" s="23" t="s">
         <v>440</v>
       </c>
-      <c r="D32" s="23" t="s">
+      <c r="D36" s="23" t="s">
         <v>443</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E36" s="23">
         <v>1</v>
       </c>
-      <c r="F32" s="23" t="s">
+      <c r="F36" s="23" t="s">
         <v>414</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="I36" s="10" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="23" t="s">
+    <row r="37" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="C37" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="23" t="s">
+      <c r="D37" s="23" t="s">
         <v>443</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E37" s="23">
         <v>1</v>
       </c>
-      <c r="F33" s="23" t="s">
+      <c r="F37" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I33" s="10"/>
-    </row>
-    <row r="34" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
+      <c r="I37" s="10"/>
+    </row>
+    <row r="38" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C38" s="10" t="s">
         <v>439</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D38" s="10" t="s">
         <v>442</v>
       </c>
-      <c r="F34" s="23" t="s">
+      <c r="F38" s="23" t="s">
         <v>414</v>
       </c>
-      <c r="H34" s="10" t="b">
+      <c r="H38" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I34" s="10" t="s">
+      <c r="I38" s="10" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
+    <row r="39" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C39" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D39" s="10" t="s">
         <v>443</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F39" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="I35" s="10" t="s">
+      <c r="I39" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="10" t="s">
+    <row r="40" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C40" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D40" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H36" s="10" t="b">
+      <c r="H40" s="10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
+    <row r="41" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C41" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D41" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H37" s="10" t="b">
+      <c r="H41" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I37" s="10" t="s">
+      <c r="I41" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="18" t="s">
+    <row r="42" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C42" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D42" s="18" t="s">
         <v>443</v>
       </c>
-      <c r="E38" s="18">
+      <c r="E42" s="18">
         <v>1</v>
       </c>
-      <c r="F38" s="18" t="s">
+      <c r="F42" s="18" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H40" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>443</v>
-      </c>
-      <c r="E41" s="18">
-        <v>1</v>
-      </c>
-      <c r="F41" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="9">
-        <v>1</v>
-      </c>
-      <c r="I42" s="9" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H43" s="9" t="b">
+      <c r="E43" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>442</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H44" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="I44" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="9" t="s">
+    </row>
+    <row r="45" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>442</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="H45" s="9" t="b">
+      <c r="C45" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>443</v>
+      </c>
+      <c r="E45" s="18">
         <v>1</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2815,13 +2809,16 @@
         <v>22</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H46" s="9" t="b">
+        <v>7</v>
+      </c>
+      <c r="E46" s="9">
         <v>1</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2829,10 +2826,10 @@
         <v>22</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="H47" s="9" t="b">
         <v>1</v>
@@ -2840,97 +2837,97 @@
     </row>
     <row r="48" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>443</v>
-      </c>
-      <c r="E48" s="9">
+        <v>442</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H48" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="F48" s="9" t="s">
-        <v>14</v>
-      </c>
       <c r="I48" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E49" s="9">
+        <v>62</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H49" s="9" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>443</v>
-      </c>
-      <c r="E50" s="9">
+        <v>38</v>
+      </c>
+      <c r="H50" s="9" t="b">
         <v>1</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I50" s="9" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" s="9">
+        <v>38</v>
+      </c>
+      <c r="H51" s="9" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>7</v>
+        <v>443</v>
+      </c>
+      <c r="E52" s="9">
+        <v>1</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="I52" s="9" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>465</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>443</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>415</v>
-      </c>
-      <c r="H53" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2939,283 +2936,348 @@
         <v>10</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H54" s="9" t="b">
+        <v>443</v>
+      </c>
+      <c r="E54" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="B55" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="D55" s="25"/>
-      <c r="I55" s="18" t="s">
-        <v>427</v>
+      <c r="F54" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I54" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>410</v>
+        <v>10</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>443</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>410</v>
-      </c>
-      <c r="H56" s="9" t="b">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="I56" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>410</v>
+        <v>10</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>78</v>
+        <v>465</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>410</v>
-      </c>
-      <c r="G57" s="9" t="s">
-        <v>76</v>
+        <v>415</v>
       </c>
       <c r="H57" s="9" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="18" t="s">
-        <v>432</v>
-      </c>
-      <c r="C58" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D58" s="18" t="s">
-        <v>443</v>
-      </c>
-      <c r="E58" s="18">
+    <row r="58" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H58" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="F58" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="9" t="s">
-        <v>432</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E59" s="9">
-        <v>1</v>
+    </row>
+    <row r="59" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="D59" s="25"/>
+      <c r="I59" s="18" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="H60" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H61" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="18" t="s">
         <v>432</v>
       </c>
-      <c r="C60" s="9" t="s">
-        <v>433</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C61" s="18" t="s">
+      <c r="C62" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D61" s="18" t="s">
+      <c r="D62" s="18" t="s">
         <v>443</v>
       </c>
-      <c r="E61" s="18">
+      <c r="E62" s="18">
         <v>1</v>
       </c>
-      <c r="F61" s="18" t="s">
+      <c r="F62" s="18" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62" s="9">
-        <v>1</v>
-      </c>
-      <c r="I62" s="9" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
-        <v>63</v>
+        <v>432</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H63" s="9" t="b">
+      <c r="E63" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C65" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>443</v>
+      </c>
+      <c r="E65" s="18">
+        <v>1</v>
+      </c>
+      <c r="F65" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" s="9">
+        <v>1</v>
+      </c>
+      <c r="I66" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H67" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D64" s="9" t="s">
+      <c r="D68" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H64" s="9" t="b">
+      <c r="H68" s="9" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="9" t="s">
+    <row r="69" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C69" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D65" s="9" t="s">
+      <c r="D69" s="9" t="s">
         <v>442</v>
       </c>
-      <c r="F65" s="9" t="s">
+      <c r="F69" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H65" s="9" t="b">
+      <c r="H69" s="9" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="19" t="s">
+    <row r="70" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="19" t="s">
         <v>35</v>
-      </c>
-      <c r="B66" s="19" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B67" s="19" t="s">
-        <v>415</v>
-      </c>
-      <c r="I67" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B68" s="22" t="s">
-        <v>415</v>
-      </c>
-      <c r="D68" s="21"/>
-    </row>
-    <row r="69" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B69" s="19" t="s">
-        <v>415</v>
-      </c>
-      <c r="D69" s="20"/>
-    </row>
-    <row r="70" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="20" t="s">
-        <v>409</v>
       </c>
       <c r="B70" s="19" t="s">
         <v>415</v>
       </c>
-      <c r="D70" s="20"/>
     </row>
     <row r="71" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="20" t="s">
-        <v>66</v>
+      <c r="A71" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="B71" s="19" t="s">
         <v>415</v>
       </c>
-      <c r="D71" s="20"/>
-    </row>
-    <row r="72" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="19" t="s">
+      <c r="I71" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B72" s="22" t="s">
         <v>415</v>
       </c>
-      <c r="B72" s="20"/>
-      <c r="D72" s="20"/>
-      <c r="I72" s="19" t="s">
+      <c r="D72" s="21"/>
+    </row>
+    <row r="73" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B73" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="D73" s="20"/>
+    </row>
+    <row r="74" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="20" t="s">
+        <v>409</v>
+      </c>
+      <c r="B74" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="D74" s="20"/>
+    </row>
+    <row r="75" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="D75" s="20"/>
+    </row>
+    <row r="76" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="B76" s="20"/>
+      <c r="D76" s="20"/>
+      <c r="I76" s="19" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="73" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="14" t="s">
+    <row r="77" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="14" t="s">
         <v>415</v>
       </c>
-      <c r="C73" s="14" t="s">
+      <c r="C77" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D73" s="14" t="s">
+      <c r="D77" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E73" s="14">
+      <c r="E77" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="14" t="s">
+    <row r="78" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="14" t="s">
         <v>415</v>
       </c>
-      <c r="C74" s="14" t="s">
+      <c r="C78" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D74" s="14" t="s">
+      <c r="D78" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E74" s="14">
+      <c r="E78" s="14">
         <v>2</v>
       </c>
-      <c r="H74" s="14" t="b">
+      <c r="H78" s="14" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J71" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
+  <autoFilter ref="A1:J75" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fix: refback for ref
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/cohort_catalogue.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/cohort_catalogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/IdeaProjects/emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C15A798-357B-5740-B429-7D909D7E6373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B13F7C-5556-5A4F-96CF-1AEAAC0AB908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <sheet name="HarmonizationStatus" sheetId="7" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">molgenis!$A$1:$J$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">molgenis!$A$1:$J$60</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="471">
   <si>
     <t>name</t>
   </si>
@@ -1518,6 +1518,15 @@
   </si>
   <si>
     <t>file</t>
+  </si>
+  <si>
+    <t>harmonisations</t>
+  </si>
+  <si>
+    <t>codes</t>
+  </si>
+  <si>
+    <t>variables</t>
   </si>
 </sst>
 </file>
@@ -2048,11 +2057,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E080B8D-E59C-EC4A-8043-87277F816BB8}">
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2441,32 +2450,33 @@
         <v>434</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
+    <row r="24" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>468</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>438</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B25" s="17" t="s">
         <v>414</v>
       </c>
-      <c r="I24" s="17" t="s">
+      <c r="I25" s="17" t="s">
         <v>430</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>443</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2474,13 +2484,16 @@
         <v>24</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H26" s="11" t="b">
-        <v>1</v>
+        <v>443</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2488,19 +2501,13 @@
         <v>24</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>443</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>409</v>
+        <v>7</v>
       </c>
       <c r="H27" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2508,16 +2515,19 @@
         <v>24</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>442</v>
+        <v>3</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>443</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H28" s="11" t="b">
         <v>1</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2525,19 +2535,16 @@
         <v>24</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>443</v>
+        <v>43</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>442</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>8</v>
+        <v>410</v>
       </c>
       <c r="H29" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="I29" s="11" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2545,13 +2552,19 @@
         <v>24</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>7</v>
+        <v>443</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="H30" s="11" t="b">
         <v>1</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2559,16 +2572,13 @@
         <v>24</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>7</v>
       </c>
       <c r="H31" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="I31" s="11" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2576,19 +2586,16 @@
         <v>24</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>444</v>
+        <v>16</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>443</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>432</v>
+        <v>7</v>
       </c>
       <c r="H32" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="I32" s="8" t="s">
-        <v>431</v>
+      <c r="I32" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2596,7 +2603,7 @@
         <v>24</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>443</v>
@@ -2608,52 +2615,52 @@
         <v>1</v>
       </c>
       <c r="I33" s="8" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="H34" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
+    <row r="35" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
         <v>408</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B35" s="17" t="s">
         <v>414</v>
       </c>
-      <c r="I34" s="17" t="s">
+      <c r="I35" s="17" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
+    <row r="36" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C36" s="11" t="s">
         <v>403</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D36" s="11" t="s">
         <v>443</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F36" s="11" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="23" t="s">
-        <v>440</v>
-      </c>
-      <c r="D36" s="23" t="s">
-        <v>443</v>
-      </c>
-      <c r="E36" s="23">
-        <v>1</v>
-      </c>
-      <c r="F36" s="23" t="s">
-        <v>414</v>
-      </c>
-      <c r="I36" s="10" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.2">
@@ -2661,7 +2668,7 @@
         <v>30</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>60</v>
+        <v>440</v>
       </c>
       <c r="D37" s="23" t="s">
         <v>443</v>
@@ -2670,45 +2677,51 @@
         <v>1</v>
       </c>
       <c r="F37" s="23" t="s">
+        <v>414</v>
+      </c>
+      <c r="H37" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>443</v>
+      </c>
+      <c r="E38" s="23">
+        <v>1</v>
+      </c>
+      <c r="F38" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I37" s="10"/>
-    </row>
-    <row r="38" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>439</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="F38" s="23" t="s">
-        <v>414</v>
-      </c>
-      <c r="H38" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>441</v>
-      </c>
+      <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>31</v>
+        <v>439</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>35</v>
+        <v>442</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>414</v>
+      </c>
+      <c r="H39" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>33</v>
+        <v>441</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -2716,13 +2729,16 @@
         <v>30</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H40" s="10" t="b">
-        <v>1</v>
+        <v>443</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -2730,7 +2746,7 @@
         <v>30</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>20</v>
@@ -2738,39 +2754,39 @@
       <c r="H41" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I41" s="10" t="s">
+    </row>
+    <row r="42" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H42" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="18" t="s">
+    <row r="43" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C43" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D42" s="18" t="s">
+      <c r="D43" s="18" t="s">
         <v>443</v>
       </c>
-      <c r="E42" s="18">
+      <c r="E43" s="18">
         <v>1</v>
       </c>
-      <c r="F42" s="18" t="s">
+      <c r="F43" s="18" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="9">
-        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2778,47 +2794,44 @@
         <v>25</v>
       </c>
       <c r="C44" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D45" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H44" s="9" t="b">
+      <c r="H45" s="9" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="18" t="s">
+    <row r="46" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="C46" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="18" t="s">
+      <c r="D46" s="18" t="s">
         <v>443</v>
       </c>
-      <c r="E45" s="18">
+      <c r="E46" s="18">
         <v>1</v>
       </c>
-      <c r="F45" s="18" t="s">
+      <c r="F46" s="18" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" s="9">
-        <v>1</v>
-      </c>
-      <c r="I46" s="9" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2826,13 +2839,16 @@
         <v>22</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H47" s="9" t="b">
+      <c r="E47" s="9">
         <v>1</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2840,19 +2856,13 @@
         <v>22</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>442</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="H48" s="9" t="b">
         <v>1</v>
-      </c>
-      <c r="I48" s="9" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2860,16 +2870,19 @@
         <v>22</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>442</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="H49" s="9" t="b">
         <v>1</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2877,10 +2890,13 @@
         <v>22</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>38</v>
+        <v>442</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="H50" s="9" t="b">
         <v>1</v>
@@ -2891,7 +2907,7 @@
         <v>22</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>38</v>
@@ -2902,22 +2918,16 @@
     </row>
     <row r="52" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>443</v>
-      </c>
-      <c r="E52" s="9">
+        <v>38</v>
+      </c>
+      <c r="H52" s="9" t="b">
         <v>1</v>
-      </c>
-      <c r="F52" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I52" s="9" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2925,44 +2935,47 @@
         <v>8</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>443</v>
       </c>
       <c r="E53" s="9">
         <v>1</v>
       </c>
+      <c r="F53" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I53" s="9" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="54" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>443</v>
+        <v>0</v>
       </c>
       <c r="E54" s="9">
         <v>1</v>
       </c>
-      <c r="F54" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I54" s="9" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="55" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="F55" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C55" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E55" s="9">
-        <v>1</v>
+      <c r="G55" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2970,13 +2983,22 @@
         <v>10</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>7</v>
+        <v>443</v>
+      </c>
+      <c r="E56" s="9">
+        <v>1</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H56" s="9" t="b">
+        <v>1</v>
       </c>
       <c r="I56" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2984,15 +3006,12 @@
         <v>10</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>465</v>
+        <v>13</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>443</v>
-      </c>
-      <c r="F57" s="9" t="s">
-        <v>415</v>
-      </c>
-      <c r="H57" s="9" t="b">
+        <v>7</v>
+      </c>
+      <c r="E57" s="9">
         <v>1</v>
       </c>
     </row>
@@ -3001,109 +3020,118 @@
         <v>10</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H58" s="9" t="b">
+        <v>7</v>
+      </c>
+      <c r="I58" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="H59" s="9" t="b">
         <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="B59" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="D59" s="25"/>
-      <c r="I59" s="18" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
-        <v>410</v>
+        <v>10</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>443</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>410</v>
+        <v>42</v>
       </c>
       <c r="H60" s="9" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="9" t="s">
+    <row r="61" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="18" t="s">
         <v>410</v>
       </c>
-      <c r="C61" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>438</v>
-      </c>
-      <c r="F61" s="9" t="s">
+      <c r="B61" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="D61" s="25"/>
+      <c r="I61" s="18" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="G61" s="9" t="s">
+      <c r="C62" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="H61" s="9" t="b">
+      <c r="D62" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="H62" s="9" t="b">
         <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="18" t="s">
-        <v>432</v>
-      </c>
-      <c r="C62" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D62" s="18" t="s">
-        <v>443</v>
-      </c>
-      <c r="E62" s="18">
-        <v>1</v>
-      </c>
-      <c r="F62" s="18" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
-        <v>432</v>
+        <v>410</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E63" s="9">
+        <v>438</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H63" s="9" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
-        <v>432</v>
+        <v>410</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>433</v>
+        <v>470</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>38</v>
+        <v>438</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H64" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="18" t="s">
-        <v>63</v>
+        <v>432</v>
       </c>
       <c r="C65" s="18" t="s">
         <v>15</v>
@@ -3120,7 +3148,7 @@
     </row>
     <row r="66" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
-        <v>63</v>
+        <v>432</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>0</v>
@@ -3131,36 +3159,33 @@
       <c r="E66" s="9">
         <v>1</v>
       </c>
-      <c r="I66" s="9" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="67" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C67" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H67" s="9" t="b">
+      <c r="C68" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="18" t="s">
+        <v>443</v>
+      </c>
+      <c r="E68" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H68" s="9" t="b">
-        <v>1</v>
+      <c r="F68" s="18" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3168,116 +3193,161 @@
         <v>63</v>
       </c>
       <c r="C69" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="9">
+        <v>1</v>
+      </c>
+      <c r="I69" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H70" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H71" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C72" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D69" s="9" t="s">
+      <c r="D72" s="9" t="s">
         <v>442</v>
       </c>
-      <c r="F69" s="9" t="s">
+      <c r="F72" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H69" s="9" t="b">
+      <c r="H72" s="9" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="19" t="s">
+    <row r="73" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="19" t="s">
         <v>35</v>
-      </c>
-      <c r="B70" s="19" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B71" s="19" t="s">
-        <v>415</v>
-      </c>
-      <c r="I71" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B72" s="22" t="s">
-        <v>415</v>
-      </c>
-      <c r="D72" s="21"/>
-    </row>
-    <row r="73" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="20" t="s">
-        <v>28</v>
       </c>
       <c r="B73" s="19" t="s">
         <v>415</v>
       </c>
-      <c r="D73" s="20"/>
     </row>
     <row r="74" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="20" t="s">
-        <v>409</v>
+      <c r="A74" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="B74" s="19" t="s">
         <v>415</v>
       </c>
-      <c r="D74" s="20"/>
-    </row>
-    <row r="75" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="20" t="s">
+      <c r="I74" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B75" s="22" t="s">
+        <v>415</v>
+      </c>
+      <c r="D75" s="21"/>
+    </row>
+    <row r="76" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B76" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="D76" s="20"/>
+    </row>
+    <row r="77" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="20" t="s">
+        <v>409</v>
+      </c>
+      <c r="B77" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="D77" s="20"/>
+    </row>
+    <row r="78" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B75" s="19" t="s">
+      <c r="B78" s="19" t="s">
         <v>415</v>
       </c>
-      <c r="D75" s="20"/>
-    </row>
-    <row r="76" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="19" t="s">
+      <c r="D78" s="20"/>
+    </row>
+    <row r="79" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="19" t="s">
         <v>415</v>
       </c>
-      <c r="B76" s="20"/>
-      <c r="D76" s="20"/>
-      <c r="I76" s="19" t="s">
+      <c r="B79" s="20"/>
+      <c r="D79" s="20"/>
+      <c r="I79" s="19" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="77" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="14" t="s">
+    <row r="80" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="14" t="s">
         <v>415</v>
       </c>
-      <c r="C77" s="14" t="s">
+      <c r="C80" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D77" s="14" t="s">
+      <c r="D80" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E77" s="14">
+      <c r="E80" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="14" t="s">
+    <row r="81" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="14" t="s">
         <v>415</v>
       </c>
-      <c r="C78" s="14" t="s">
+      <c r="C81" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D78" s="14" t="s">
+      <c r="D81" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E78" s="14">
+      <c r="E81" s="14">
         <v>2</v>
       </c>
-      <c r="H78" s="14" t="b">
+      <c r="H81" s="14" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J75" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
+  <autoFilter ref="A1:J78" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fix: composite key cannot contain nullable columns
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/cohort_catalogue.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/cohort_catalogue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/IdeaProjects/emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B13F7C-5556-5A4F-96CF-1AEAAC0AB908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EC8BBD-F9CF-294A-A9F0-32E66C0B8820}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="6" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="472">
   <si>
     <t>name</t>
   </si>
@@ -1527,6 +1527,9 @@
   </si>
   <si>
     <t>variables</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -2059,9 +2062,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E080B8D-E59C-EC4A-8043-87277F816BB8}">
   <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H37" sqref="H37"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2406,9 +2409,6 @@
       <c r="F21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="11" t="b">
-        <v>1</v>
-      </c>
       <c r="I21" s="11" t="s">
         <v>436</v>
       </c>
@@ -2679,9 +2679,6 @@
       <c r="F37" s="23" t="s">
         <v>414</v>
       </c>
-      <c r="H37" s="23" t="b">
-        <v>1</v>
-      </c>
       <c r="I37" s="10" t="s">
         <v>437</v>
       </c>
@@ -2993,9 +2990,6 @@
       </c>
       <c r="F56" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="H56" s="9" t="b">
-        <v>1</v>
       </c>
       <c r="I56" s="9" t="s">
         <v>19</v>
@@ -5760,7 +5754,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1048576"/>
+      <selection activeCell="B11" sqref="B11:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6145,6 +6139,12 @@
       <c r="A11" t="s">
         <v>370</v>
       </c>
+      <c r="B11" t="s">
+        <v>370</v>
+      </c>
+      <c r="C11" t="s">
+        <v>471</v>
+      </c>
       <c r="D11" t="s">
         <v>383</v>
       </c>
@@ -6173,6 +6173,12 @@
       <c r="A12" t="s">
         <v>370</v>
       </c>
+      <c r="B12" t="s">
+        <v>370</v>
+      </c>
+      <c r="C12" t="s">
+        <v>471</v>
+      </c>
       <c r="D12" t="s">
         <v>384</v>
       </c>
@@ -6200,6 +6206,12 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>370</v>
+      </c>
+      <c r="B13" t="s">
+        <v>370</v>
+      </c>
+      <c r="C13" t="s">
+        <v>471</v>
       </c>
       <c r="D13" t="s">
         <v>385</v>
@@ -6433,10 +6445,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B958AC-AE9C-6646-926B-247F9F6B40B5}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6485,6 +6497,14 @@
         <v>417</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>370</v>
+      </c>
+      <c r="B6" t="s">
+        <v>471</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6494,8 +6514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552128E9-1EC3-674C-BB17-36DDC2F16F66}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6599,7 +6619,7 @@
         <v>347</v>
       </c>
       <c r="F3" s="27" t="str">
-        <f t="shared" ref="F3:F13" si="1">E3</f>
+        <f t="shared" ref="F3:G13" si="1">E3</f>
         <v>CHOP</v>
       </c>
       <c r="G3" s="27" t="str">
@@ -6905,6 +6925,13 @@
         <f t="shared" si="1"/>
         <v>NINFEA</v>
       </c>
+      <c r="G11" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v>NINFEA</v>
+      </c>
+      <c r="H11" t="s">
+        <v>471</v>
+      </c>
       <c r="I11" t="s">
         <v>383</v>
       </c>
@@ -6939,6 +6966,13 @@
         <f t="shared" si="1"/>
         <v>NINFEA</v>
       </c>
+      <c r="G12" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v>NINFEA</v>
+      </c>
+      <c r="H12" t="s">
+        <v>471</v>
+      </c>
       <c r="I12" t="s">
         <v>384</v>
       </c>
@@ -6972,6 +7006,13 @@
       <c r="F13" s="27" t="str">
         <f t="shared" si="1"/>
         <v>NINFEA</v>
+      </c>
+      <c r="G13" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v>NINFEA</v>
+      </c>
+      <c r="H13" t="s">
+        <v>471</v>
       </c>
       <c r="I13" t="s">
         <v>385</v>

</xml_diff>

<commit_message>
feat: ref_array foreign key can now overlap with ref foreign keys (i.e. they become linked to each other)
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/cohort_catalogue.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/cohort_catalogue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/IdeaProjects/emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98EE6D8-F286-0842-9D98-F12ABD384E9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9C6E50-4904-1749-8F0D-D921294D1AAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23880" windowHeight="20540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28760" windowHeight="20540" activeTab="6" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Variable" sheetId="3" r:id="rId4"/>
     <sheet name="RepeatedVariable" sheetId="12" r:id="rId5"/>
     <sheet name="Table" sheetId="13" r:id="rId6"/>
-    <sheet name="Harmonization" sheetId="4" r:id="rId7"/>
+    <sheet name="VariableHarmonization" sheetId="4" r:id="rId7"/>
     <sheet name="CodeList" sheetId="8" r:id="rId8"/>
     <sheet name="Code" sheetId="9" r:id="rId9"/>
     <sheet name="Format" sheetId="6" r:id="rId10"/>
@@ -39,52 +39,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Morris Swertz</author>
-  </authors>
-  <commentList>
-    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{1D849659-0ABF-1446-9CFE-C292473BDDF5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Morris Swertz:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">will be automatically repeated to length of sourceVariables
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="513">
   <si>
     <t>name</t>
   </si>
@@ -1611,9 +1567,6 @@
     <t>collectionName,codeListName,codeLabel</t>
   </si>
   <si>
-    <t>source,targetCollection,targetTable,targetVariable</t>
-  </si>
-  <si>
     <t>harmonisationsSource,harmonisationTargetCollection,harmonisationTargetTable,harmonisationTargetVariable</t>
   </si>
   <si>
@@ -1648,13 +1601,22 @@
   </si>
   <si>
     <t>targetCollection,targetTable</t>
+  </si>
+  <si>
+    <t>sourceCollection,targetCollection,targetTable,targetVariable</t>
+  </si>
+  <si>
+    <t>soc_born_father,soc_born_mother</t>
+  </si>
+  <si>
+    <t>table1,table1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1703,19 +1665,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -2173,9 +2122,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E080B8D-E59C-EC4A-8043-87277F816BB8}">
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2762,13 +2711,13 @@
         <v>433</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>498</v>
+        <v>510</v>
       </c>
       <c r="I34" s="7" t="s">
         <v>486</v>
@@ -3152,7 +3101,7 @@
         <v>59</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="H55" s="7" t="s">
         <v>478</v>
@@ -3415,7 +3364,7 @@
     </row>
     <row r="71" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>434</v>
@@ -3430,7 +3379,7 @@
         <v>23</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H71" s="24" t="s">
         <v>478</v>
@@ -3438,10 +3387,10 @@
     </row>
     <row r="72" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="C72" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>508</v>
       </c>
       <c r="E72" s="6">
         <v>1</v>
@@ -3450,7 +3399,7 @@
         <v>23</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H72" s="24" t="s">
         <v>478</v>
@@ -3458,7 +3407,7 @@
     </row>
     <row r="73" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>4</v>
@@ -3469,7 +3418,7 @@
     </row>
     <row r="74" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="25" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C74" s="25" t="s">
         <v>29</v>
@@ -3480,10 +3429,10 @@
     </row>
     <row r="75" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="18" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>434</v>
+        <v>486</v>
       </c>
       <c r="D75" s="18" t="s">
         <v>437</v>
@@ -3492,16 +3441,24 @@
         <v>1</v>
       </c>
       <c r="F75" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="K75" s="6"/>
+        <v>409</v>
+      </c>
+      <c r="G75" s="18" t="s">
+        <v>487</v>
+      </c>
+      <c r="H75" s="18" t="s">
+        <v>484</v>
+      </c>
+      <c r="K75" s="6" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="76" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="18" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>486</v>
+        <v>56</v>
       </c>
       <c r="D76" s="18" t="s">
         <v>437</v>
@@ -3510,84 +3467,76 @@
         <v>1</v>
       </c>
       <c r="F76" s="18" t="s">
-        <v>409</v>
-      </c>
-      <c r="G76" s="18" t="s">
-        <v>487</v>
-      </c>
-      <c r="H76" s="18" t="s">
-        <v>484</v>
-      </c>
-      <c r="K76" s="6" t="s">
-        <v>432</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="K76" s="6"/>
     </row>
     <row r="77" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="18" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>485</v>
+        <v>28</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>436</v>
-      </c>
-      <c r="F77" s="18" t="s">
-        <v>409</v>
-      </c>
-      <c r="G77" s="20" t="s">
-        <v>488</v>
-      </c>
-      <c r="H77" s="18" t="s">
-        <v>484</v>
-      </c>
-      <c r="J77" s="6" t="b">
-        <v>1</v>
+        <v>437</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>467</v>
       </c>
       <c r="K77" s="6" t="s">
-        <v>435</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="18" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>28</v>
+        <v>466</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>437</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>467</v>
+        <v>468</v>
+      </c>
+      <c r="J78" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="K78" s="6" t="s">
-        <v>30</v>
+        <v>469</v>
       </c>
     </row>
     <row r="79" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="18" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>466</v>
+        <v>485</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>437</v>
-      </c>
-      <c r="F79" s="6" t="s">
-        <v>468</v>
+        <v>436</v>
+      </c>
+      <c r="F79" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="G79" s="20" t="s">
+        <v>488</v>
+      </c>
+      <c r="H79" s="18" t="s">
+        <v>484</v>
       </c>
       <c r="J79" s="6" t="b">
         <v>1</v>
       </c>
       <c r="K79" s="6" t="s">
-        <v>469</v>
+        <v>435</v>
       </c>
     </row>
     <row r="80" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="18" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>4</v>
@@ -3601,7 +3550,7 @@
     </row>
     <row r="81" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="18" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>29</v>
@@ -6608,10 +6557,10 @@
         <v>21</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>501</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -6767,135 +6716,126 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552128E9-1EC3-674C-BB17-36DDC2F16F66}">
-  <dimension ref="A1:J15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552128E9-1EC3-674C-BB17-36DDC2F16F66}">
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="15" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="2"/>
-    <col min="9" max="9" width="80.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="255.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="31.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="80.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>434</v>
+        <v>502</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>503</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>504</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>505</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>485</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>64</v>
+      <c r="E2" s="2" t="s">
+        <v>343</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>344</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="2" t="str">
-        <f>A3</f>
-        <v>CHOP</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="2" t="str">
-        <f>A4</f>
-        <v>CHOP</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>412</v>
@@ -6904,54 +6844,50 @@
         <v>373</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" s="2" t="str">
-        <f>A6</f>
-        <v>ELFE</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>412</v>
@@ -6960,31 +6896,27 @@
         <v>375</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E7" s="2" t="str">
-        <f>A7</f>
-        <v>ELFE</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>412</v>
@@ -6993,31 +6925,27 @@
         <v>374</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="2" t="str">
-        <f>A8</f>
-        <v>GenR</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>412</v>
@@ -7026,31 +6954,27 @@
         <v>376</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="2" t="str">
-        <f>A9</f>
-        <v>GenR</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>412</v>
@@ -7059,57 +6983,53 @@
         <v>377</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>344</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="2" t="str">
-        <f>A11</f>
-        <v>NINFEA</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>447</v>
@@ -7118,31 +7038,27 @@
         <v>378</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="2" t="str">
-        <f>A12</f>
-        <v>NINFEA</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>447</v>
@@ -7151,31 +7067,27 @@
         <v>379</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="2" t="str">
-        <f>A13</f>
-        <v>NINFEA</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>447</v>
@@ -7184,58 +7096,53 @@
         <v>380</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    </row>
+    <row r="15" spans="1:9" s="21" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>342</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="21" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
-        <v>342</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="21" t="s">
+        <v>390</v>
+      </c>
       <c r="F15" s="2"/>
-      <c r="H15" s="21" t="s">
-        <v>390</v>
-      </c>
-      <c r="I15" s="22" t="s">
+      <c r="H15" s="22" t="s">
         <v>413</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>